<commit_message>
complete compute MODIS value for each county
</commit_message>
<xml_diff>
--- a/Step_1_Process_Yearbook_Data/02_Digitized_data/河南_2009_仅小麦产量.xlsx
+++ b/Step_1_Process_Yearbook_Data/02_Digitized_data/河南_2009_仅小麦产量.xlsx
@@ -1,24 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangj\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wangj\Desktop\Agricultural_production\Step_1_Process_Yearbook_Data\02_Digitized_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76716486-FE8B-4C82-886C-C8B8A3D2E762}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{833603A1-7F31-4C5A-A8E6-F9CC20FCEA1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="9465" yWindow="3045" windowWidth="15855" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId2"/>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <definedNames>
     <definedName name="\a">#N/A</definedName>
     <definedName name="\d">#REF!</definedName>
@@ -36,14 +32,6 @@
     <definedName name="철구사업본부">#REF!</definedName>
   </definedNames>
   <calcPr calcId="114210"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -378,24 +366,24 @@
     <t>地区</t>
   </si>
   <si>
-    <t>产量</t>
+    <t>小麦产量</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="10">
-    <numFmt numFmtId="169" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="171" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="0_);[Red]\(0\)"/>
-    <numFmt numFmtId="184" formatCode="#.00"/>
-    <numFmt numFmtId="186" formatCode="#."/>
-    <numFmt numFmtId="187" formatCode="m\o\n\th\ d\,\ yyyy"/>
-    <numFmt numFmtId="197" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="198" formatCode="mmm\ dd\,\ yy"/>
-    <numFmt numFmtId="199" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="200" formatCode="mm/dd/yy_)"/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="166" formatCode="0_);[Red]\(0\)"/>
+    <numFmt numFmtId="167" formatCode="#.00"/>
+    <numFmt numFmtId="168" formatCode="#."/>
+    <numFmt numFmtId="169" formatCode="m\o\n\th\ d\,\ yyyy"/>
+    <numFmt numFmtId="170" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="171" formatCode="mmm\ dd\,\ yy"/>
+    <numFmt numFmtId="172" formatCode="_(&quot;$&quot;* #,##0.0_);_(&quot;$&quot;* \(#,##0.0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="173" formatCode="mm/dd/yy_)"/>
   </numFmts>
   <fonts count="34">
     <font>
@@ -889,7 +877,7 @@
   </borders>
   <cellStyleXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="186" fontId="2" fillId="0" borderId="0">
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
@@ -947,10 +935,10 @@
     <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="187" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="169" fontId="5" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="184" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="167" fontId="5" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
@@ -959,14 +947,14 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="7" fillId="0" borderId="0">
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="186" fontId="7" fillId="0" borderId="0">
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="186" fontId="5" fillId="0" borderId="9">
+    <xf numFmtId="168" fontId="5" fillId="0" borderId="9">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="38" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -974,15 +962,15 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="186" fontId="23" fillId="0" borderId="0">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="168" fontId="23" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="186" fontId="23" fillId="0" borderId="0">
+    <xf numFmtId="168" fontId="23" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="171" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1007,7 +995,7 @@
     <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="23" fillId="0" borderId="0">
+    <xf numFmtId="168" fontId="23" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1035,8 +1023,8 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="199" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="200" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="172" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="173" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1059,15 +1047,15 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="197" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="198" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="170" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="171" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="30" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1108,75 +1096,75 @@
     </xf>
   </cellXfs>
   <cellStyles count="69">
-    <cellStyle name="_29" xfId="1"/>
-    <cellStyle name="0,0_x000a__x000a_NA_x000a__x000a_" xfId="2"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="3"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="4"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="5"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="6"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="7"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="8"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="9"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="10"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="11"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="12"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="13"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="14"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="15"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="16"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="17"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="18"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="19"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="20"/>
-    <cellStyle name="Date" xfId="21"/>
-    <cellStyle name="Fixed" xfId="22"/>
-    <cellStyle name="Header1" xfId="23"/>
-    <cellStyle name="Header2" xfId="24"/>
-    <cellStyle name="Heading1" xfId="25"/>
-    <cellStyle name="Heading2" xfId="26"/>
+    <cellStyle name="_29" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="0,0_x000a__x000a_NA_x000a__x000a_" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="9" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="11" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="12" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="13" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="14" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="15" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="16" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="17" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="18" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="19" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="20" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Date" xfId="21" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Fixed" xfId="22" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Header1" xfId="23" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="Header2" xfId="24" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Heading1" xfId="25" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Heading2" xfId="26" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Style 1" xfId="27"/>
+    <cellStyle name="Style 1" xfId="27" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
     <cellStyle name="Total" xfId="28" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="콤마 [0]_BOILER-CO1" xfId="29"/>
-    <cellStyle name="콤마_BOILER-CO1" xfId="30"/>
-    <cellStyle name="통화 [0]_BOILER-CO1" xfId="31"/>
-    <cellStyle name="통화_BOILER-CO1" xfId="32"/>
-    <cellStyle name="표준_0N-HANDLING " xfId="33"/>
-    <cellStyle name="千位[0]_GetDateDialog" xfId="34"/>
-    <cellStyle name="千位_GetDateDialog" xfId="35"/>
-    <cellStyle name="千分位" xfId="36"/>
-    <cellStyle name="千分位[0]" xfId="37"/>
-    <cellStyle name="千分位_ 白土" xfId="38"/>
-    <cellStyle name="好" xfId="39"/>
-    <cellStyle name="差" xfId="40"/>
-    <cellStyle name="强调文字颜色 1" xfId="41"/>
-    <cellStyle name="强调文字颜色 2" xfId="42"/>
-    <cellStyle name="强调文字颜色 3" xfId="43"/>
-    <cellStyle name="强调文字颜色 4" xfId="44"/>
-    <cellStyle name="强调文字颜色 5" xfId="45"/>
-    <cellStyle name="强调文字颜色 6" xfId="46"/>
-    <cellStyle name="普通" xfId="47"/>
-    <cellStyle name="标题" xfId="48"/>
-    <cellStyle name="标题 1" xfId="49"/>
-    <cellStyle name="标题 2" xfId="50"/>
-    <cellStyle name="标题 3" xfId="51"/>
-    <cellStyle name="标题 4" xfId="52"/>
-    <cellStyle name="样式 1" xfId="53"/>
-    <cellStyle name="检查单元格" xfId="54"/>
-    <cellStyle name="汇总" xfId="55"/>
-    <cellStyle name="注释" xfId="56"/>
-    <cellStyle name="烹拳 [0]_97MBO" xfId="57"/>
-    <cellStyle name="烹拳_97MBO" xfId="58"/>
-    <cellStyle name="解释性文本" xfId="59"/>
-    <cellStyle name="警告文本" xfId="60"/>
-    <cellStyle name="计算" xfId="61"/>
-    <cellStyle name="输入" xfId="62"/>
-    <cellStyle name="输出" xfId="63"/>
-    <cellStyle name="适中" xfId="64"/>
-    <cellStyle name="钎霖_laroux" xfId="65"/>
-    <cellStyle name="链接单元格" xfId="66"/>
-    <cellStyle name="霓付 [0]_97MBO" xfId="67"/>
-    <cellStyle name="霓付_97MBO" xfId="68"/>
+    <cellStyle name="콤마 [0]_BOILER-CO1" xfId="29" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="콤마_BOILER-CO1" xfId="30" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="통화 [0]_BOILER-CO1" xfId="31" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="통화_BOILER-CO1" xfId="32" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="표준_0N-HANDLING " xfId="33" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="千位[0]_GetDateDialog" xfId="34" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="千位_GetDateDialog" xfId="35" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="千分位" xfId="36" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="千分位[0]" xfId="37" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="千分位_ 白土" xfId="38" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="好" xfId="39" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="差" xfId="40" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="强调文字颜色 1" xfId="41" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="强调文字颜色 2" xfId="42" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="强调文字颜色 3" xfId="43" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="强调文字颜色 4" xfId="44" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="强调文字颜色 5" xfId="45" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="普通" xfId="47" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="标题" xfId="48" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="标题 1" xfId="49" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="标题 2" xfId="50" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="标题 3" xfId="51" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="标题 4" xfId="52" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="样式 1" xfId="53" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="检查单元格" xfId="54" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="汇总" xfId="55" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="注释" xfId="56" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="烹拳 [0]_97MBO" xfId="57" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="烹拳_97MBO" xfId="58" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="解释性文本" xfId="59" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="警告文本" xfId="60" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="计算" xfId="61" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="输入" xfId="62" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="输出" xfId="63" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="适中" xfId="64" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="钎霖_laroux" xfId="65" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="链接单元格" xfId="66" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="霓付 [0]_97MBO" xfId="67" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="霓付_97MBO" xfId="68" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1189,38 +1177,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="22-1"/>
-      <sheetName val="22-2"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="22-11"/>
-      <sheetName val="22-11(1)"/>
-      <sheetName val="22-11(2)"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1519,11 +1475,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N190"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A118" sqref="A118:IV118"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -3993,6 +3949,47 @@
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="A110:XFD110"/>
+    <mergeCell ref="A115:XFD115"/>
+    <mergeCell ref="A116:XFD116"/>
+    <mergeCell ref="A117:XFD117"/>
+    <mergeCell ref="A118:XFD118"/>
+    <mergeCell ref="A111:XFD111"/>
+    <mergeCell ref="A112:XFD112"/>
+    <mergeCell ref="A113:XFD113"/>
+    <mergeCell ref="A114:XFD114"/>
+    <mergeCell ref="A123:XFD123"/>
+    <mergeCell ref="A124:XFD124"/>
+    <mergeCell ref="A125:XFD125"/>
+    <mergeCell ref="A126:XFD126"/>
+    <mergeCell ref="A119:XFD119"/>
+    <mergeCell ref="A120:XFD120"/>
+    <mergeCell ref="A121:XFD121"/>
+    <mergeCell ref="A122:XFD122"/>
+    <mergeCell ref="A131:XFD131"/>
+    <mergeCell ref="A132:XFD132"/>
+    <mergeCell ref="A133:XFD133"/>
+    <mergeCell ref="A134:XFD134"/>
+    <mergeCell ref="A127:XFD127"/>
+    <mergeCell ref="A128:XFD128"/>
+    <mergeCell ref="A129:XFD129"/>
+    <mergeCell ref="A130:XFD130"/>
+    <mergeCell ref="A139:XFD139"/>
+    <mergeCell ref="A140:XFD140"/>
+    <mergeCell ref="A141:XFD141"/>
+    <mergeCell ref="A142:XFD142"/>
+    <mergeCell ref="A135:XFD135"/>
+    <mergeCell ref="A136:XFD136"/>
+    <mergeCell ref="A137:XFD137"/>
+    <mergeCell ref="A138:XFD138"/>
+    <mergeCell ref="A147:XFD147"/>
+    <mergeCell ref="A148:XFD148"/>
+    <mergeCell ref="A149:XFD149"/>
+    <mergeCell ref="A150:XFD150"/>
+    <mergeCell ref="A143:XFD143"/>
+    <mergeCell ref="A144:XFD144"/>
+    <mergeCell ref="A145:XFD145"/>
+    <mergeCell ref="A146:XFD146"/>
     <mergeCell ref="A155:XFD155"/>
     <mergeCell ref="A156:XFD156"/>
     <mergeCell ref="A157:XFD157"/>
@@ -4001,47 +3998,6 @@
     <mergeCell ref="A152:XFD152"/>
     <mergeCell ref="A153:XFD153"/>
     <mergeCell ref="A154:XFD154"/>
-    <mergeCell ref="A147:XFD147"/>
-    <mergeCell ref="A148:XFD148"/>
-    <mergeCell ref="A149:XFD149"/>
-    <mergeCell ref="A150:XFD150"/>
-    <mergeCell ref="A143:XFD143"/>
-    <mergeCell ref="A144:XFD144"/>
-    <mergeCell ref="A145:XFD145"/>
-    <mergeCell ref="A146:XFD146"/>
-    <mergeCell ref="A139:XFD139"/>
-    <mergeCell ref="A140:XFD140"/>
-    <mergeCell ref="A141:XFD141"/>
-    <mergeCell ref="A142:XFD142"/>
-    <mergeCell ref="A135:XFD135"/>
-    <mergeCell ref="A136:XFD136"/>
-    <mergeCell ref="A137:XFD137"/>
-    <mergeCell ref="A138:XFD138"/>
-    <mergeCell ref="A131:XFD131"/>
-    <mergeCell ref="A132:XFD132"/>
-    <mergeCell ref="A133:XFD133"/>
-    <mergeCell ref="A134:XFD134"/>
-    <mergeCell ref="A127:XFD127"/>
-    <mergeCell ref="A128:XFD128"/>
-    <mergeCell ref="A129:XFD129"/>
-    <mergeCell ref="A130:XFD130"/>
-    <mergeCell ref="A123:XFD123"/>
-    <mergeCell ref="A124:XFD124"/>
-    <mergeCell ref="A125:XFD125"/>
-    <mergeCell ref="A126:XFD126"/>
-    <mergeCell ref="A119:XFD119"/>
-    <mergeCell ref="A120:XFD120"/>
-    <mergeCell ref="A121:XFD121"/>
-    <mergeCell ref="A122:XFD122"/>
-    <mergeCell ref="A115:XFD115"/>
-    <mergeCell ref="A116:XFD116"/>
-    <mergeCell ref="A117:XFD117"/>
-    <mergeCell ref="A118:XFD118"/>
-    <mergeCell ref="A111:XFD111"/>
-    <mergeCell ref="A112:XFD112"/>
-    <mergeCell ref="A113:XFD113"/>
-    <mergeCell ref="A114:XFD114"/>
-    <mergeCell ref="A110:XFD110"/>
   </mergeCells>
   <phoneticPr fontId="29" type="noConversion"/>
   <pageMargins left="0.66929135735579359" right="0.66929131042300249" top="0.82677161599707416" bottom="0.82677170986265647" header="0" footer="0"/>

</xml_diff>